<commit_message>
Creacion de tabla e ingreso del primer reporte
</commit_message>
<xml_diff>
--- a/Reporte_diario.xlsx
+++ b/Reporte_diario.xlsx
@@ -1,26 +1,67 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22827"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\Residencia\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BFFEB9A-C626-420F-B87A-10E62C335CA2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+  <si>
+    <t>H-total</t>
+  </si>
+  <si>
+    <t>No. Día</t>
+  </si>
+  <si>
+    <t>Fecha</t>
+  </si>
+  <si>
+    <t>Descipción</t>
+  </si>
+  <si>
+    <t>Horas Total</t>
+  </si>
+  <si>
+    <t>Restan</t>
+  </si>
+  <si>
+    <t>Curso de Git, Github/ Instalacion de SQL SERVER / Conexión a la base de datos ACC MEX</t>
+  </si>
+  <si>
+    <t>Dias de trabajo</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -28,13 +69,38 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -49,8 +115,28 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -330,13 +416,192 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="B2:H23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" style="4"/>
+    <col min="5" max="5" width="82.140625" customWidth="1"/>
+    <col min="6" max="6" width="6.42578125" customWidth="1"/>
+    <col min="7" max="7" width="14.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H2">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B3" s="5">
+        <v>1</v>
+      </c>
+      <c r="C3" s="7">
+        <f ca="1">TODAY()</f>
+        <v>44013</v>
+      </c>
+      <c r="D3" s="5">
+        <v>6</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H3">
+        <f>H2 - (SUM(D3:D23))</f>
+        <v>494</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B4" s="6"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="3"/>
+      <c r="G4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H4">
+        <f>SUM(B3:B23)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="2"/>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="3"/>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="2"/>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B8" s="6"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="3"/>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="2"/>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="3"/>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="2"/>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="3"/>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="2"/>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B14" s="6"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="3"/>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="2"/>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B16" s="6"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="3"/>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B17" s="5"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="2"/>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B18" s="6"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="3"/>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="2"/>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B20" s="6"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="3"/>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B21" s="5"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="2"/>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B22" s="6"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="3"/>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B23" s="5"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="2"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Reporte del día 2
</commit_message>
<xml_diff>
--- a/Reporte_diario.xlsx
+++ b/Reporte_diario.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\Residencia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BFFEB9A-C626-420F-B87A-10E62C335CA2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FFCAC70-8A93-4CAE-8E62-3E0F887BEE28}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,14 +31,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>H-total</t>
   </si>
   <si>
-    <t>No. Día</t>
-  </si>
-  <si>
     <t>Fecha</t>
   </si>
   <si>
@@ -55,13 +52,22 @@
   </si>
   <si>
     <t>Dias de trabajo</t>
+  </si>
+  <si>
+    <t>Día</t>
+  </si>
+  <si>
+    <t>Hrs acomuladas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Documentación de 27 tablas de la base de datos </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -76,8 +82,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="2" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -102,8 +115,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -111,11 +130,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -135,6 +169,17 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -417,186 +462,261 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:H23"/>
+  <dimension ref="B2:J23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="2" max="2" width="4.42578125" customWidth="1"/>
     <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.140625" style="4"/>
     <col min="5" max="5" width="82.140625" customWidth="1"/>
     <col min="6" max="6" width="6.42578125" customWidth="1"/>
     <col min="7" max="7" width="14.7109375" customWidth="1"/>
+    <col min="10" max="10" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>1</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>2</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="H2">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B3" s="5">
+        <v>2</v>
+      </c>
+      <c r="G2" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="H2" s="12">
+        <f xml:space="preserve"> (SUM(D3:D25))</f>
+        <v>16</v>
+      </c>
+      <c r="J2" s="9"/>
+    </row>
+    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B3" s="10">
         <v>1</v>
       </c>
       <c r="C3" s="7">
-        <f ca="1">TODAY()</f>
-        <v>44013</v>
+        <v>44014</v>
       </c>
       <c r="D3" s="5">
         <v>6</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H3">
-        <f>H2 - (SUM(D3:D23))</f>
-        <v>494</v>
-      </c>
-    </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="6"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="3"/>
-      <c r="G4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="H4">
-        <f>SUM(B3:B23)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B5" s="5"/>
+      <c r="G3" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="H3" s="12">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B4" s="10">
+        <f>(IF(C4="",0,1+B3))</f>
+        <v>2</v>
+      </c>
+      <c r="C4" s="8">
+        <v>44015</v>
+      </c>
+      <c r="D4" s="6">
+        <v>10</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="H4" s="12">
+        <f>H3 - (SUM(D3:D23))</f>
+        <v>484</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B5" s="10" t="str">
+        <f>(IF(C5="","",1+B4))</f>
+        <v/>
+      </c>
       <c r="C5" s="5"/>
       <c r="D5" s="5"/>
       <c r="E5" s="2"/>
-    </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B6" s="6"/>
+      <c r="G5" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="H5" s="12">
+        <f>MAX(B3:B23)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B6" s="10" t="str">
+        <f t="shared" ref="B6:B23" si="0">(IF(C6="","",1+B5))</f>
+        <v/>
+      </c>
       <c r="C6" s="6"/>
       <c r="D6" s="6"/>
       <c r="E6" s="3"/>
     </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B7" s="5"/>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B7" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
       <c r="E7" s="2"/>
     </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B8" s="6"/>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B8" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="C8" s="6"/>
       <c r="D8" s="6"/>
       <c r="E8" s="3"/>
     </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B9" s="5"/>
+    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B9" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
       <c r="E9" s="2"/>
     </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B10" s="6"/>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B10" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="C10" s="6"/>
       <c r="D10" s="6"/>
       <c r="E10" s="3"/>
     </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B11" s="5"/>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B11" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="C11" s="5"/>
       <c r="D11" s="5"/>
       <c r="E11" s="2"/>
     </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B12" s="6"/>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B12" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="C12" s="6"/>
       <c r="D12" s="6"/>
       <c r="E12" s="3"/>
     </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B13" s="5"/>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B13" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="C13" s="5"/>
       <c r="D13" s="5"/>
       <c r="E13" s="2"/>
     </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B14" s="6"/>
+    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B14" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="C14" s="6"/>
       <c r="D14" s="6"/>
       <c r="E14" s="3"/>
     </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B15" s="5"/>
+    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B15" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
       <c r="E15" s="2"/>
     </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B16" s="6"/>
+    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B16" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="C16" s="6"/>
       <c r="D16" s="6"/>
       <c r="E16" s="3"/>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B17" s="5"/>
+      <c r="B17" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="C17" s="5"/>
       <c r="D17" s="5"/>
       <c r="E17" s="2"/>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B18" s="6"/>
+      <c r="B18" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="C18" s="6"/>
       <c r="D18" s="6"/>
       <c r="E18" s="3"/>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B19" s="5"/>
+      <c r="B19" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="C19" s="5"/>
       <c r="D19" s="5"/>
       <c r="E19" s="2"/>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B20" s="6"/>
+      <c r="B20" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="3"/>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B21" s="5"/>
+      <c r="B21" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="C21" s="5"/>
       <c r="D21" s="5"/>
       <c r="E21" s="2"/>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B22" s="6"/>
+      <c r="B22" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="C22" s="6"/>
       <c r="D22" s="6"/>
       <c r="E22" s="3"/>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B23" s="5"/>
+      <c r="B23" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="C23" s="5"/>
       <c r="D23" s="5"/>
       <c r="E23" s="2"/>

</xml_diff>

<commit_message>
Reporte del día 4
</commit_message>
<xml_diff>
--- a/Reporte_diario.xlsx
+++ b/Reporte_diario.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\Residencia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{702C58C1-23C3-40A5-BFD7-85CB973FA202}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56214653-7629-4AC9-ACAD-9D4FC34679E6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4560" yWindow="1260" windowWidth="13680" windowHeight="8055" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>H-total</t>
   </si>
@@ -63,7 +63,10 @@
     <t xml:space="preserve">Documentación de 27 tablas de la base de datos </t>
   </si>
   <si>
-    <t>Documentacion de 30 Procediminetos Almacenados de la base de datos ACC MEX</t>
+    <t>Documentacion de 20 Procediminetos Almacenados de la base de datos ACC MEX</t>
+  </si>
+  <si>
+    <t>Documentacion de 24 Procediminetos Almacenados de la base de datos ACC MEX</t>
   </si>
 </sst>
 </file>
@@ -468,7 +471,7 @@
   <dimension ref="B2:J23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -500,7 +503,7 @@
       </c>
       <c r="H2" s="12">
         <f xml:space="preserve"> (SUM(D3:D25))</f>
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="J2" s="9"/>
     </row>
@@ -543,7 +546,7 @@
       </c>
       <c r="H4" s="12">
         <f>H3 - (SUM(D3:D23))</f>
-        <v>478</v>
+        <v>472</v>
       </c>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.25">
@@ -558,24 +561,30 @@
         <v>6</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G5" s="11" t="s">
         <v>6</v>
       </c>
       <c r="H5" s="12">
         <f>MAX(B3:B23)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B6" s="10" t="str">
+      <c r="B6" s="10">
         <f t="shared" ref="B6:B23" si="0">(IF(C6="","",1+B5))</f>
-        <v/>
-      </c>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="3"/>
+        <v>4</v>
+      </c>
+      <c r="C6" s="7">
+        <v>44019</v>
+      </c>
+      <c r="D6" s="6">
+        <v>6</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B7" s="10" t="str">

</xml_diff>

<commit_message>
Correccion de Procedimientos almacenados
</commit_message>
<xml_diff>
--- a/Reporte_diario.xlsx
+++ b/Reporte_diario.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\Residencia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56214653-7629-4AC9-ACAD-9D4FC34679E6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D976C2C-FC46-42A1-B20D-26BE09CB7077}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4560" yWindow="1260" windowWidth="13680" windowHeight="8055" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>H-total</t>
   </si>
@@ -67,6 +67,9 @@
   </si>
   <si>
     <t>Documentacion de 24 Procediminetos Almacenados de la base de datos ACC MEX</t>
+  </si>
+  <si>
+    <t>Correccion de 30 Procedimientos almacenados de la base de datos ACC MEX</t>
   </si>
 </sst>
 </file>
@@ -96,7 +99,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -124,6 +127,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -155,7 +164,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -174,9 +183,6 @@
     <xf numFmtId="14" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -188,6 +194,13 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -470,8 +483,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:J23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" zoomScale="94" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -498,17 +511,17 @@
       <c r="E2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="13" t="s">
+      <c r="G2" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="12">
+      <c r="H2" s="11">
         <f xml:space="preserve"> (SUM(D3:D25))</f>
-        <v>28</v>
-      </c>
-      <c r="J2" s="9"/>
+        <v>32</v>
+      </c>
+      <c r="J2" s="8"/>
     </row>
     <row r="3" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B3" s="10">
+      <c r="B3" s="9">
         <v>1</v>
       </c>
       <c r="C3" s="7">
@@ -520,37 +533,37 @@
       <c r="E3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="11" t="s">
+      <c r="G3" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="H3" s="12">
+      <c r="H3" s="11">
         <v>500</v>
       </c>
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B4" s="10">
+      <c r="B4" s="9">
         <f>(IF(C4="",0,1+B3))</f>
         <v>2</v>
       </c>
-      <c r="C4" s="8">
+      <c r="C4" s="13">
         <v>44015</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D4" s="14">
         <v>10</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="13" t="s">
+      <c r="G4" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="H4" s="12">
+      <c r="H4" s="11">
         <f>H3 - (SUM(D3:D23))</f>
-        <v>472</v>
+        <v>468</v>
       </c>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B5" s="10">
+      <c r="B5" s="9">
         <f>(IF(C5="","",1+B4))</f>
         <v>3</v>
       </c>
@@ -563,49 +576,55 @@
       <c r="E5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G5" s="11" t="s">
+      <c r="G5" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="H5" s="12">
+      <c r="H5" s="11">
         <f>MAX(B3:B23)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B6" s="10">
+      <c r="B6" s="9">
         <f t="shared" ref="B6:B23" si="0">(IF(C6="","",1+B5))</f>
         <v>4</v>
       </c>
-      <c r="C6" s="7">
+      <c r="C6" s="13">
         <v>44019</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D6" s="14">
         <v>6</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="E6" s="15" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B7" s="10" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="2"/>
+      <c r="B7" s="9">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="C7" s="7">
+        <v>44021</v>
+      </c>
+      <c r="D7" s="5">
+        <v>4</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B8" s="10" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="3"/>
+      <c r="B8" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="C8" s="14"/>
+      <c r="D8" s="14"/>
+      <c r="E8" s="15"/>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B9" s="10" t="str">
+      <c r="B9" s="9" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -614,7 +633,7 @@
       <c r="E9" s="2"/>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B10" s="10" t="str">
+      <c r="B10" s="9" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -623,7 +642,7 @@
       <c r="E10" s="3"/>
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B11" s="10" t="str">
+      <c r="B11" s="9" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -632,7 +651,7 @@
       <c r="E11" s="2"/>
     </row>
     <row r="12" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B12" s="10" t="str">
+      <c r="B12" s="9" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -641,7 +660,7 @@
       <c r="E12" s="3"/>
     </row>
     <row r="13" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B13" s="10" t="str">
+      <c r="B13" s="9" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -650,7 +669,7 @@
       <c r="E13" s="2"/>
     </row>
     <row r="14" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B14" s="10" t="str">
+      <c r="B14" s="9" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -659,7 +678,7 @@
       <c r="E14" s="3"/>
     </row>
     <row r="15" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B15" s="10" t="str">
+      <c r="B15" s="9" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -668,7 +687,7 @@
       <c r="E15" s="2"/>
     </row>
     <row r="16" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B16" s="10" t="str">
+      <c r="B16" s="9" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -677,7 +696,7 @@
       <c r="E16" s="3"/>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B17" s="10" t="str">
+      <c r="B17" s="9" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -686,7 +705,7 @@
       <c r="E17" s="2"/>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B18" s="10" t="str">
+      <c r="B18" s="9" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -695,7 +714,7 @@
       <c r="E18" s="3"/>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B19" s="10" t="str">
+      <c r="B19" s="9" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -704,7 +723,7 @@
       <c r="E19" s="2"/>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B20" s="10" t="str">
+      <c r="B20" s="9" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -713,7 +732,7 @@
       <c r="E20" s="3"/>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B21" s="10" t="str">
+      <c r="B21" s="9" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -722,7 +741,7 @@
       <c r="E21" s="2"/>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B22" s="10" t="str">
+      <c r="B22" s="9" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -731,7 +750,7 @@
       <c r="E22" s="3"/>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B23" s="10" t="str">
+      <c r="B23" s="9" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>

</xml_diff>

<commit_message>
Reporte del dia 7
</commit_message>
<xml_diff>
--- a/Reporte_diario.xlsx
+++ b/Reporte_diario.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23001"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\Residencia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D976C2C-FC46-42A1-B20D-26BE09CB7077}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0C7A181-7820-4F4A-9B6C-691EB1C2469A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>H-total</t>
   </si>
@@ -63,13 +63,19 @@
     <t xml:space="preserve">Documentación de 27 tablas de la base de datos </t>
   </si>
   <si>
-    <t>Documentacion de 20 Procediminetos Almacenados de la base de datos ACC MEX</t>
-  </si>
-  <si>
-    <t>Documentacion de 24 Procediminetos Almacenados de la base de datos ACC MEX</t>
-  </si>
-  <si>
-    <t>Correccion de 30 Procedimientos almacenados de la base de datos ACC MEX</t>
+    <t>Diseño de vistas para la aplicación "Pantallas" en Adobe Illustrator (MenuPrincipal)</t>
+  </si>
+  <si>
+    <t>Analisis de codigo, pruebas de codigo original, toma de decisión para rehacer el sistema de "Pantallas</t>
+  </si>
+  <si>
+    <t>Documentacion de 24 Procediminetos Almacenados de la base de datos ACC MEX TEST</t>
+  </si>
+  <si>
+    <t>Documentacion de 20 Procediminetos Almacenados de la base de datos ACC MEX TEST</t>
+  </si>
+  <si>
+    <t>Correccion de 30 Procedimientos almacenados de la base de datos ACC MEX TEST</t>
   </si>
 </sst>
 </file>
@@ -484,7 +490,7 @@
   <dimension ref="B2:J23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="94" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -492,7 +498,7 @@
     <col min="2" max="2" width="4.42578125" customWidth="1"/>
     <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.140625" style="4"/>
-    <col min="5" max="5" width="82.140625" customWidth="1"/>
+    <col min="5" max="5" width="88.5703125" customWidth="1"/>
     <col min="6" max="6" width="6.42578125" customWidth="1"/>
     <col min="7" max="7" width="14.7109375" customWidth="1"/>
     <col min="10" max="10" width="10.7109375" bestFit="1" customWidth="1"/>
@@ -516,7 +522,7 @@
       </c>
       <c r="H2" s="11">
         <f xml:space="preserve"> (SUM(D3:D25))</f>
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="J2" s="8"/>
     </row>
@@ -549,7 +555,7 @@
         <v>44015</v>
       </c>
       <c r="D4" s="14">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="E4" s="15" t="s">
         <v>9</v>
@@ -559,7 +565,7 @@
       </c>
       <c r="H4" s="11">
         <f>H3 - (SUM(D3:D23))</f>
-        <v>468</v>
+        <v>462</v>
       </c>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.25">
@@ -574,14 +580,14 @@
         <v>6</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G5" s="10" t="s">
         <v>6</v>
       </c>
       <c r="H5" s="11">
         <f>MAX(B3:B23)</f>
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.25">
@@ -596,7 +602,7 @@
         <v>6</v>
       </c>
       <c r="E6" s="15" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.25">
@@ -611,26 +617,38 @@
         <v>4</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B8" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="C8" s="14"/>
-      <c r="D8" s="14"/>
-      <c r="E8" s="15"/>
+      <c r="B8" s="9">
+        <f>(IF(C8="","",1+B7))</f>
+        <v>6</v>
+      </c>
+      <c r="C8" s="13">
+        <v>44027</v>
+      </c>
+      <c r="D8" s="14">
+        <v>4</v>
+      </c>
+      <c r="E8" s="15" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B9" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="2"/>
+      <c r="B9" s="9">
+        <f>(IF(C9="","",1+B8))</f>
+        <v>7</v>
+      </c>
+      <c r="C9" s="7">
+        <v>44026</v>
+      </c>
+      <c r="D9" s="5">
+        <v>6</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B10" s="9" t="str">

</xml_diff>

<commit_message>
Reporte del día 8
</commit_message>
<xml_diff>
--- a/Reporte_diario.xlsx
+++ b/Reporte_diario.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\Residencia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0C7A181-7820-4F4A-9B6C-691EB1C2469A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9F9674E-346F-434B-8EF0-CB141A06933A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>H-total</t>
   </si>
@@ -76,6 +76,9 @@
   </si>
   <si>
     <t>Correccion de 30 Procedimientos almacenados de la base de datos ACC MEX TEST</t>
+  </si>
+  <si>
+    <t>Creacion de diseño de vistas para par el programa "Pantallas"</t>
   </si>
 </sst>
 </file>
@@ -490,7 +493,7 @@
   <dimension ref="B2:J23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="94" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -522,7 +525,7 @@
       </c>
       <c r="H2" s="11">
         <f xml:space="preserve"> (SUM(D3:D25))</f>
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="J2" s="8"/>
     </row>
@@ -565,7 +568,7 @@
       </c>
       <c r="H4" s="11">
         <f>H3 - (SUM(D3:D23))</f>
-        <v>462</v>
+        <v>455</v>
       </c>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.25">
@@ -587,7 +590,7 @@
       </c>
       <c r="H5" s="11">
         <f>MAX(B3:B23)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.25">
@@ -651,13 +654,19 @@
       </c>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B10" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="3"/>
+      <c r="B10" s="9">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="C10" s="7">
+        <v>44027</v>
+      </c>
+      <c r="D10" s="6">
+        <v>7</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B11" s="9" t="str">

</xml_diff>